<commit_message>
adding extreme pathway support
</commit_message>
<xml_diff>
--- a/input_test/Glycolysis_Grasp_isoenzymes.xlsx
+++ b/input_test/Glycolysis_Grasp_isoenzymes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicow/Documents/Metabolomics/GRASP_inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicow/Documents/GRASP/input_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468AD0B0-472E-1343-8307-21D8AE3B6E26}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BCE1C1-F474-2F41-88ED-06804A482B25}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="731" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="731" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="25" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="135">
   <si>
     <t>adp</t>
   </si>
@@ -420,9 +420,6 @@
     <t>PFK</t>
   </si>
   <si>
-    <t>mixedInhibitionUniUni</t>
-  </si>
-  <si>
     <t>Substrate Order</t>
   </si>
   <si>
@@ -442,6 +439,12 @@
   </si>
   <si>
     <t>f6p_c atp_c</t>
+  </si>
+  <si>
+    <t>orderedTerBi</t>
+  </si>
+  <si>
+    <t>uniUni</t>
   </si>
 </sst>
 </file>
@@ -1377,7 +1380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
@@ -51107,8 +51110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="55.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -51135,10 +51138,10 @@
         <v>19</v>
       </c>
       <c r="C1" s="77" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="78" t="s">
         <v>127</v>
-      </c>
-      <c r="D1" s="78" t="s">
-        <v>128</v>
       </c>
       <c r="E1" s="77" t="s">
         <v>84</v>
@@ -51173,10 +51176,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D2" s="54" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H2" s="54" t="s">
         <v>121</v>
@@ -51199,10 +51202,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D3" s="54" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H3" s="54" t="s">
         <v>92</v>
@@ -51219,16 +51222,10 @@
         <v>47</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>126</v>
-      </c>
-      <c r="F4" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="G4" s="54" t="s">
-        <v>97</v>
+        <v>134</v>
       </c>
       <c r="J4" s="55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="55">
         <v>2</v>
@@ -51242,10 +51239,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F5" s="54"/>
       <c r="G5" s="54"/>
@@ -51271,10 +51268,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D6" s="54" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H6" s="54" t="s">
         <v>93</v>
@@ -51297,10 +51294,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D7" s="54" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H7" s="54" t="s">
         <v>122</v>
@@ -51323,7 +51320,7 @@
         <v>97</v>
       </c>
       <c r="D8" s="54" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J8" s="55">
         <v>1</v>
@@ -51337,7 +51334,7 @@
         <v>72</v>
       </c>
       <c r="B9" s="55" t="s">
-        <v>3</v>
+        <v>133</v>
       </c>
       <c r="J9" s="55">
         <v>1</v>
@@ -51397,7 +51394,7 @@
       <c r="H12" s="54"/>
       <c r="I12" s="54"/>
       <c r="J12" s="55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" s="55">
         <v>2</v>
@@ -51416,7 +51413,7 @@
       <c r="H13" s="54"/>
       <c r="I13" s="54"/>
       <c r="J13" s="55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="55">
         <v>2</v>

</xml_diff>